<commit_message>
fixed 0 for benefits
</commit_message>
<xml_diff>
--- a/app/output/analise-19-12-25-vr.xlsx
+++ b/app/output/analise-19-12-25-vr.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,75 +473,70 @@
       </c>
       <c r="F1" s="2" t="inlineStr">
         <is>
-          <t>Resultado</t>
+          <t>Alerta</t>
         </is>
       </c>
       <c r="G1" s="2" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>DEMITIDO?</t>
         </is>
       </c>
       <c r="H1" s="2" t="inlineStr">
         <is>
-          <t>DEMITIDO?</t>
+          <t>AVISO PRÉVIO?</t>
         </is>
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>AVISO PRÉVIO?</t>
+          <t>SITUAÇÃO</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
         <is>
-          <t>SITUAÇÃO</t>
+          <t>Cargo</t>
         </is>
       </c>
       <c r="K1" s="2" t="inlineStr">
         <is>
-          <t>Cargo</t>
+          <t>Escala</t>
         </is>
       </c>
       <c r="L1" s="2" t="inlineStr">
         <is>
-          <t>Escala</t>
+          <t>Qtd. Dias Trabalhados</t>
         </is>
       </c>
       <c r="M1" s="2" t="inlineStr">
         <is>
-          <t>Qtd. Dias Trabalhados</t>
+          <t>Falta Injustificada</t>
         </is>
       </c>
       <c r="N1" s="2" t="inlineStr">
         <is>
-          <t>Falta Injustificada</t>
+          <t>Falta Justificada</t>
         </is>
       </c>
       <c r="O1" s="2" t="inlineStr">
         <is>
-          <t>Falta Justificada</t>
+          <t>Falta Abonada</t>
         </is>
       </c>
       <c r="P1" s="2" t="inlineStr">
         <is>
-          <t>Falta Abonada</t>
+          <t>INSS</t>
         </is>
       </c>
       <c r="Q1" s="2" t="inlineStr">
         <is>
-          <t>INSS</t>
+          <t>Suspensão</t>
         </is>
       </c>
       <c r="R1" s="2" t="inlineStr">
         <is>
-          <t>Suspensão</t>
+          <t>Folga Trabalhada</t>
         </is>
       </c>
       <c r="S1" s="2" t="inlineStr">
-        <is>
-          <t>Folga Trabalhada</t>
-        </is>
-      </c>
-      <c r="T1" s="2" t="inlineStr">
         <is>
           <t>Folga Trabalhada Cash</t>
         </is>
@@ -564,9 +559,17 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>394.44</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -576,26 +579,24 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>ENCARREGADO</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>ENCARREGADO</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
           <t>6x1 Folga Fixa</t>
         </is>
       </c>
+      <c r="L2" t="n">
+        <v>3</v>
+      </c>
       <c r="M2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N2" t="n">
         <v>0</v>
@@ -613,9 +614,6 @@
         <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -634,11 +632,19 @@
         <v>269.88</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>195.8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>74.07999999999998</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>valor localizado em datas diversas</t>
+        </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>o valor 195.80 foi localizado na data 02/12/2025</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -648,26 +654,24 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
       <c r="M3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N3" t="n">
         <v>0</v>
@@ -685,9 +689,6 @@
         <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -708,9 +709,17 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
+      <c r="E4" t="n">
+        <v>269.88</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -720,24 +729,22 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>ZELADOR</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>ZELADOR</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
           <t>12x36</t>
         </is>
       </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
@@ -757,9 +764,6 @@
         <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -780,9 +784,17 @@
       <c r="D5" t="n">
         <v>0</v>
       </c>
+      <c r="E5" t="n">
+        <v>207.6</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -792,26 +804,24 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
       <c r="M5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -829,9 +839,6 @@
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -852,9 +859,17 @@
       <c r="D6" t="n">
         <v>0</v>
       </c>
+      <c r="E6" t="n">
+        <v>186.84</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -864,26 +879,24 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L6" t="n">
+        <v>2</v>
+      </c>
       <c r="M6" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
         <v>0</v>
@@ -901,9 +914,6 @@
         <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -924,9 +934,17 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="n">
+        <v>166.08</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -936,26 +954,24 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
       <c r="M7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
@@ -973,9 +989,6 @@
         <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -996,9 +1009,17 @@
       <c r="D8" t="n">
         <v>0</v>
       </c>
+      <c r="E8" t="n">
+        <v>456.72</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -1008,26 +1029,24 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUX SERVICOS GERAIS</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>AUX SERVICOS GERAIS</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
           <t>5x1</t>
         </is>
       </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
       <c r="M8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -1045,9 +1064,6 @@
         <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1068,9 +1084,17 @@
       <c r="D9" t="n">
         <v>0</v>
       </c>
+      <c r="E9" t="n">
+        <v>456.72</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1080,26 +1104,24 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUX SERVICOS GERAIS</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>AUX SERVICOS GERAIS</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
           <t>5x1</t>
         </is>
       </c>
+      <c r="L9" t="n">
+        <v>1</v>
+      </c>
       <c r="M9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
@@ -1117,9 +1139,6 @@
         <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1140,9 +1159,17 @@
       <c r="D10" t="n">
         <v>0</v>
       </c>
+      <c r="E10" t="n">
+        <v>456.72</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1152,26 +1179,24 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUX SERVICOS GERAIS</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>AUX SERVICOS GERAIS</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
           <t>5x1</t>
         </is>
       </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
       <c r="M10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -1189,9 +1214,6 @@
         <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
-      </c>
-      <c r="T10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1212,9 +1234,17 @@
       <c r="D11" t="n">
         <v>0</v>
       </c>
+      <c r="E11" t="n">
+        <v>456.72</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1224,26 +1254,24 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUX SERVICOS GERAIS</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>AUX SERVICOS GERAIS</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
           <t>5x1</t>
         </is>
       </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
@@ -1261,9 +1289,6 @@
         <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1284,9 +1309,17 @@
       <c r="D12" t="n">
         <v>0</v>
       </c>
+      <c r="E12" t="n">
+        <v>456.72</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1296,26 +1329,24 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>PLANTÃO</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>PLANTÃO</t>
+          <t>AUX SERVICOS GERAIS</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>AUX SERVICOS GERAIS</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
           <t>5x1</t>
         </is>
       </c>
+      <c r="L12" t="n">
+        <v>1</v>
+      </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -1333,9 +1364,6 @@
         <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1356,9 +1384,17 @@
       <c r="D13" t="n">
         <v>0</v>
       </c>
+      <c r="E13" t="n">
+        <v>145.32</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1368,24 +1404,22 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
       <c r="M13" t="n">
         <v>0</v>
       </c>
@@ -1405,9 +1439,6 @@
         <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>0</v>
-      </c>
-      <c r="T13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1428,9 +1459,17 @@
       <c r="D14" t="n">
         <v>0</v>
       </c>
+      <c r="E14" t="n">
+        <v>332.16</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1440,24 +1479,22 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AGENTE HIGIENIZACAO</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>AGENTE HIGIENIZACAO</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
       <c r="M14" t="n">
         <v>0</v>
       </c>
@@ -1477,9 +1514,6 @@
         <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1500,9 +1534,17 @@
       <c r="D15" t="n">
         <v>0</v>
       </c>
+      <c r="E15" t="n">
+        <v>332.16</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1512,24 +1554,22 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
       <c r="M15" t="n">
         <v>0</v>
       </c>
@@ -1549,9 +1589,6 @@
         <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>0</v>
-      </c>
-      <c r="T15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1572,9 +1609,17 @@
       <c r="D16" t="n">
         <v>0</v>
       </c>
+      <c r="E16" t="n">
+        <v>311.4</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1584,24 +1629,22 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L16" t="n">
+        <v>0</v>
+      </c>
       <c r="M16" t="n">
         <v>0</v>
       </c>
@@ -1621,9 +1664,6 @@
         <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1644,9 +1684,17 @@
       <c r="D17" t="n">
         <v>0</v>
       </c>
+      <c r="E17" t="n">
+        <v>311.4</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1656,24 +1704,22 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>AUXILIAR DE LIMPEZA</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>AUXILIAR DE LIMPEZA</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
       <c r="M17" t="n">
         <v>0</v>
       </c>
@@ -1693,9 +1739,6 @@
         <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>0</v>
-      </c>
-      <c r="T17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1716,9 +1759,17 @@
       <c r="D18" t="n">
         <v>0</v>
       </c>
+      <c r="E18" t="n">
+        <v>269.88</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1728,24 +1779,22 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>ENCARREGADO(A)</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>ENCARREGADO(A)</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L18" t="n">
+        <v>0</v>
+      </c>
       <c r="M18" t="n">
         <v>0</v>
       </c>
@@ -1765,9 +1814,6 @@
         <v>0</v>
       </c>
       <c r="S18" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1788,9 +1834,17 @@
       <c r="D19" t="n">
         <v>0</v>
       </c>
+      <c r="E19" t="n">
+        <v>300</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>nada encontrado</t>
+        </is>
+      </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>nada encontrado</t>
+          <t>ATIVO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1800,24 +1854,22 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>ATIVO</t>
+          <t>EFETIVO</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>EFETIVO</t>
+          <t>PREPARADOR DE DADOS</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>PREPARADOR DE DADOS</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
           <t>5x2 SDF Folga</t>
         </is>
       </c>
+      <c r="L19" t="n">
+        <v>0</v>
+      </c>
       <c r="M19" t="n">
         <v>0</v>
       </c>
@@ -1837,9 +1889,6 @@
         <v>0</v>
       </c>
       <c r="S19" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>